<commit_message>
added KMR DN 100
</commit_message>
<xml_diff>
--- a/F-Heat_QGIS/data/costs.xlsx
+++ b/F-Heat_QGIS/data/costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lars_Goray\AppData\Roaming\QGIS\QGIS3\profiles\default\python\plugins\heat_net_tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43FF3EE-3C3A-4B02-8E47-3E66BEC8BB40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44837EC4-33D8-494B-BCA4-5978BBA7774E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9684" xr2:uid="{CB187417-A205-4705-9999-9FBFDE89F3A6}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="71">
   <si>
     <t>PEX* / KMR**</t>
   </si>
@@ -171,9 +171,6 @@
     <t>- DN 80 - 100 ==&gt; PEX-Einzelrohr</t>
   </si>
   <si>
-    <t xml:space="preserve">- DN 125 - 300 ==&gt; KMR-Einzelrohr </t>
-  </si>
-  <si>
     <t>- Preisbasis gültig bis 31.12.2024 (es ist mit einem jährlichen Teuerungszuschlag in Höhe von 8%  zu rechnen)</t>
   </si>
   <si>
@@ -238,6 +235,12 @@
   </si>
   <si>
     <t>DN 100 (PEX 110*10mm)*</t>
+  </si>
+  <si>
+    <t>DN 100 (114,3*3,2mm)**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- DN 100 - 300 ==&gt; KMR-Einzelrohr </t>
   </si>
 </sst>
 </file>
@@ -583,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -684,6 +687,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -857,13 +862,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>89647</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2570802</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>93830</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1231,40 +1236,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>63</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1274,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45CAD31A-D488-48F9-8381-5023A1748DE7}">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
@@ -1294,103 +1299,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="69"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="66"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="64"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="66"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="64"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="66"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="66"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="68"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="62" t="s">
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="68"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="66"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="62" t="s">
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="66"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="62" t="s">
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="68"/>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A11" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="66"/>
-    </row>
-    <row r="11" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A11" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="45"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="30"/>
@@ -1400,20 +1405,20 @@
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="55"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="57"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="56"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="58"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="31"/>
@@ -1469,7 +1474,7 @@
         <v>69</v>
       </c>
       <c r="D19" s="7">
-        <f t="shared" ref="D19:D30" si="0">B19*C19</f>
+        <f t="shared" ref="D19:D31" si="0">B19*C19</f>
         <v>0</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -1573,7 +1578,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" s="4">
         <f>Zusammenfassung!G9</f>
@@ -1590,16 +1595,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" s="38" customFormat="1">
       <c r="A26" s="22" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="B26" s="4">
         <f>Zusammenfassung!G10</f>
         <v>0</v>
       </c>
       <c r="C26" s="6">
-        <v>387</v>
+        <v>315</v>
       </c>
       <c r="D26" s="7">
         <f t="shared" si="0"/>
@@ -1611,14 +1616,14 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" s="4">
         <f>Zusammenfassung!G11</f>
         <v>0</v>
       </c>
       <c r="C27" s="6">
-        <v>417</v>
+        <v>387</v>
       </c>
       <c r="D27" s="7">
         <f t="shared" si="0"/>
@@ -1630,14 +1635,14 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" s="4">
         <f>Zusammenfassung!G12</f>
         <v>0</v>
       </c>
       <c r="C28" s="6">
-        <v>559</v>
+        <v>417</v>
       </c>
       <c r="D28" s="7">
         <f t="shared" si="0"/>
@@ -1649,14 +1654,14 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="4">
         <f>Zusammenfassung!G13</f>
         <v>0</v>
       </c>
       <c r="C29" s="6">
-        <v>803</v>
+        <v>559</v>
       </c>
       <c r="D29" s="7">
         <f t="shared" si="0"/>
@@ -1667,15 +1672,15 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="23" t="s">
-        <v>7</v>
+      <c r="A30" s="22" t="s">
+        <v>6</v>
       </c>
       <c r="B30" s="4">
         <f>Zusammenfassung!G14</f>
         <v>0</v>
       </c>
       <c r="C30" s="6">
-        <v>996</v>
+        <v>803</v>
       </c>
       <c r="D30" s="7">
         <f t="shared" si="0"/>
@@ -1686,109 +1691,109 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="4">
+        <f>Zusammenfassung!G15</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="6">
+        <v>996</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="4">
-        <f>SUM(B19:B30)</f>
-        <v>0</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="7">
-        <f>SUM(D19:D30)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="29" t="s">
+      <c r="B32" s="4">
+        <f>SUM(B19:B31)</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="7">
+        <f>SUM(D19:D31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="8" t="s">
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="21" t="s">
+    <row r="37" spans="1:5">
+      <c r="A37" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B37" s="4">
         <f>Zusammenfassung!G3</f>
         <v>0</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C37" s="6">
         <v>78</v>
       </c>
-      <c r="D36" s="7">
-        <f t="shared" ref="D36:D47" si="1">B36*C36</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="4">
-        <f>Zusammenfassung!G4</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="6">
-        <v>85</v>
-      </c>
       <c r="D37" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D37:D49" si="1">B37*C37</f>
         <v>0</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:5">
       <c r="A38" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B38" s="4">
-        <f>Zusammenfassung!G5</f>
+        <f>Zusammenfassung!G4</f>
         <v>0</v>
       </c>
       <c r="C38" s="6">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="D38" s="7">
         <f t="shared" si="1"/>
@@ -1798,16 +1803,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:5">
       <c r="A39" s="21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B39" s="4">
-        <f>Zusammenfassung!G6</f>
+        <f>Zusammenfassung!G5</f>
         <v>0</v>
       </c>
       <c r="C39" s="6">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="D39" s="7">
         <f t="shared" si="1"/>
@@ -1817,16 +1822,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:5">
       <c r="A40" s="21" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B40" s="4">
-        <f>Zusammenfassung!G7</f>
+        <f>Zusammenfassung!G6</f>
         <v>0</v>
       </c>
       <c r="C40" s="6">
-        <v>210</v>
+        <v>143</v>
       </c>
       <c r="D40" s="7">
         <f t="shared" si="1"/>
@@ -1836,35 +1841,35 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:5">
       <c r="A41" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B41" s="4">
-        <f>Zusammenfassung!G8</f>
+        <f>Zusammenfassung!G7</f>
         <v>0</v>
       </c>
       <c r="C41" s="6">
-        <v>266</v>
+        <v>210</v>
       </c>
       <c r="D41" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="21" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="B42" s="4">
-        <f>Zusammenfassung!G9</f>
+        <f>Zusammenfassung!G8</f>
         <v>0</v>
       </c>
       <c r="C42" s="6">
-        <v>319</v>
+        <v>266</v>
       </c>
       <c r="D42" s="7">
         <f t="shared" si="1"/>
@@ -1874,16 +1879,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:5">
       <c r="A43" s="21" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B43" s="4">
-        <f>Zusammenfassung!G10</f>
+        <f>Zusammenfassung!G9</f>
         <v>0</v>
       </c>
       <c r="C43" s="6">
-        <v>434</v>
+        <v>319</v>
       </c>
       <c r="D43" s="7">
         <f t="shared" si="1"/>
@@ -1893,16 +1898,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="21" t="s">
-        <v>4</v>
+    <row r="44" spans="1:5" s="39" customFormat="1">
+      <c r="A44" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="B44" s="4">
-        <f>Zusammenfassung!G11</f>
+        <f>Zusammenfassung!G10</f>
         <v>0</v>
       </c>
       <c r="C44" s="6">
-        <v>472</v>
+        <v>356</v>
       </c>
       <c r="D44" s="7">
         <f t="shared" si="1"/>
@@ -1912,16 +1917,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:5">
       <c r="A45" s="21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B45" s="4">
-        <f>Zusammenfassung!G12</f>
+        <f>Zusammenfassung!G11</f>
         <v>0</v>
       </c>
       <c r="C45" s="6">
-        <v>632</v>
+        <v>434</v>
       </c>
       <c r="D45" s="7">
         <f t="shared" si="1"/>
@@ -1931,16 +1936,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:5">
       <c r="A46" s="21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B46" s="4">
-        <f>Zusammenfassung!G13</f>
+        <f>Zusammenfassung!G12</f>
         <v>0</v>
       </c>
       <c r="C46" s="6">
-        <v>900</v>
+        <v>472</v>
       </c>
       <c r="D46" s="7">
         <f t="shared" si="1"/>
@@ -1950,16 +1955,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:5">
       <c r="A47" s="21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B47" s="4">
-        <f>Zusammenfassung!G14</f>
+        <f>Zusammenfassung!G13</f>
         <v>0</v>
       </c>
       <c r="C47" s="6">
-        <v>1126</v>
+        <v>632</v>
       </c>
       <c r="D47" s="7">
         <f t="shared" si="1"/>
@@ -1968,267 +1973,245 @@
       <c r="E47" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H47" t="s">
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="4">
+        <f>Zusammenfassung!G14</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="6">
+        <v>900</v>
+      </c>
+      <c r="D48" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="4">
+        <f>Zusammenfassung!G15</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="6">
+        <v>1126</v>
+      </c>
+      <c r="D49" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="8" t="s">
+    <row r="50" spans="1:10">
+      <c r="A50" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B48" s="4">
-        <f>SUM(B36:B47)</f>
-        <v>0</v>
-      </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="7">
-        <f>SUM(D36:D47)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="14.4" thickBot="1">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-    </row>
-    <row r="50" spans="1:10" ht="15" customHeight="1">
-      <c r="A50" s="45" t="s">
+      <c r="B50" s="4">
+        <f>SUM(B37:B49)</f>
+        <v>0</v>
+      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="7">
+        <f>SUM(D37:D49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="14.4" thickBot="1">
+      <c r="A51" s="31"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+    </row>
+    <row r="52" spans="1:10" ht="15" customHeight="1">
+      <c r="A52" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B50" s="46"/>
-      <c r="C50" s="46"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="47"/>
-    </row>
-    <row r="51" spans="1:10" ht="14.4" thickBot="1">
-      <c r="A51" s="48"/>
-      <c r="B51" s="49"/>
-      <c r="C51" s="49"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="50"/>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="26" t="s">
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="49"/>
+    </row>
+    <row r="53" spans="1:10" ht="14.4" thickBot="1">
+      <c r="A53" s="50"/>
+      <c r="B53" s="51"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="52"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="G53" s="38" t="s">
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="G55" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="H53" s="39"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39"/>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54" s="25" t="s">
+      <c r="H55" s="41"/>
+      <c r="I55" s="41"/>
+      <c r="J55" s="41"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B56" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C56" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D56" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G54" s="17" t="s">
+      <c r="G56" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H54" s="17" t="s">
+      <c r="H56" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I54" s="17" t="s">
+      <c r="I56" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J56" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="J54" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="8" t="s">
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B57" s="4">
         <f>Zusammenfassung!E2</f>
         <v>0</v>
       </c>
-      <c r="C55" s="6">
+      <c r="C57" s="6">
         <v>3560</v>
       </c>
-      <c r="D55" s="7">
-        <f>B55*C55</f>
-        <v>0</v>
-      </c>
-      <c r="G55" s="8" t="s">
+      <c r="D57" s="7">
+        <f>B57*C57</f>
+        <v>0</v>
+      </c>
+      <c r="G57" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H55" s="18">
+      <c r="H57" s="18">
         <v>49</v>
       </c>
-      <c r="I55" s="33">
-        <f>Zusammenfassung!F2-B55*15</f>
-        <v>0</v>
-      </c>
-      <c r="J55" s="18">
-        <f>H55*I55</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="A56" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="4">
-        <f>Zusammenfassung!E3</f>
-        <v>0</v>
-      </c>
-      <c r="C56" s="6">
-        <v>3850</v>
-      </c>
-      <c r="D56" s="7">
-        <f t="shared" ref="D56:D61" si="2">B56*C56</f>
-        <v>0</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H56" s="18">
-        <v>54</v>
-      </c>
-      <c r="I56" s="33">
-        <f>Zusammenfassung!F3-B56*15</f>
-        <v>0</v>
-      </c>
-      <c r="J56" s="18">
-        <f>H56*I56</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A57" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" s="4">
-        <f>Zusammenfassung!E4</f>
-        <v>0</v>
-      </c>
-      <c r="C57" s="6">
-        <v>4120</v>
-      </c>
-      <c r="D57" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G57" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H57" s="18">
-        <v>63</v>
-      </c>
       <c r="I57" s="33">
-        <f>Zusammenfassung!F4-B57*15</f>
+        <f>Zusammenfassung!F2-B57*15</f>
         <v>0</v>
       </c>
       <c r="J57" s="18">
-        <f t="shared" ref="J57:J61" si="3">H57*I57</f>
+        <f>H57*I57</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B58" s="4">
-        <f>Zusammenfassung!E5</f>
+        <f>Zusammenfassung!E3</f>
         <v>0</v>
       </c>
       <c r="C58" s="6">
-        <v>4800</v>
+        <v>3850</v>
       </c>
       <c r="D58" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D58:D63" si="2">B58*C58</f>
         <v>0</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H58" s="18">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="I58" s="33">
-        <f>Zusammenfassung!F5-B58*15</f>
+        <f>Zusammenfassung!F3-B58*15</f>
         <v>0</v>
       </c>
       <c r="J58" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+        <f>H58*I58</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="14.25" customHeight="1">
       <c r="A59" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B59" s="4">
-        <f>Zusammenfassung!E6</f>
+        <f>Zusammenfassung!E4</f>
         <v>0</v>
       </c>
       <c r="C59" s="6">
-        <v>5580</v>
+        <v>4120</v>
       </c>
       <c r="D59" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H59" s="18">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="I59" s="33">
-        <f>Zusammenfassung!F6-B59*15</f>
+        <f>Zusammenfassung!F4-B59*15</f>
         <v>0</v>
       </c>
       <c r="J59" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J59:J63" si="3">H59*I59</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B60" s="4">
-        <f>Zusammenfassung!E7</f>
+        <f>Zusammenfassung!E5</f>
         <v>0</v>
       </c>
       <c r="C60" s="6">
-        <v>7200</v>
+        <v>4800</v>
       </c>
       <c r="D60" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H60" s="18">
-        <v>155</v>
+        <v>81</v>
       </c>
       <c r="I60" s="33">
-        <f>Zusammenfassung!F7-B60*15</f>
+        <f>Zusammenfassung!F5-B60*15</f>
         <v>0</v>
       </c>
       <c r="J60" s="18">
@@ -2238,27 +2221,27 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B61" s="4">
-        <f>Zusammenfassung!E8</f>
+        <f>Zusammenfassung!E6</f>
         <v>0</v>
       </c>
       <c r="C61" s="6">
-        <v>9690</v>
+        <v>5580</v>
       </c>
       <c r="D61" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H61" s="34">
-        <v>183</v>
+        <v>22</v>
+      </c>
+      <c r="H61" s="18">
+        <v>107</v>
       </c>
       <c r="I61" s="33">
-        <f>Zusammenfassung!F8-B61*15</f>
+        <f>Zusammenfassung!F6-B61*15</f>
         <v>0</v>
       </c>
       <c r="J61" s="18">
@@ -2268,216 +2251,216 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="4">
+        <f>Zusammenfassung!E7</f>
+        <v>0</v>
+      </c>
+      <c r="C62" s="6">
+        <v>7200</v>
+      </c>
+      <c r="D62" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H62" s="18">
+        <v>155</v>
+      </c>
+      <c r="I62" s="33">
+        <f>Zusammenfassung!F7-B62*15</f>
+        <v>0</v>
+      </c>
+      <c r="J62" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" s="4">
+        <f>Zusammenfassung!E8</f>
+        <v>0</v>
+      </c>
+      <c r="C63" s="6">
+        <v>9690</v>
+      </c>
+      <c r="D63" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H63" s="34">
+        <v>183</v>
+      </c>
+      <c r="I63" s="33">
+        <f>Zusammenfassung!F8-B63*15</f>
+        <v>0</v>
+      </c>
+      <c r="J63" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B62" s="4">
-        <f>SUM(B55:B61)</f>
-        <v>0</v>
-      </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="7">
-        <f>SUM(D55:D61)</f>
-        <v>0</v>
-      </c>
-      <c r="G62" s="35" t="s">
+      <c r="B64" s="4">
+        <f>SUM(B57:B63)</f>
+        <v>0</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="7">
+        <f>SUM(D57:D63)</f>
+        <v>0</v>
+      </c>
+      <c r="G64" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H62" s="36"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="37">
-        <f>SUM(J55:J61)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="31"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="27" t="s">
+      <c r="H64" s="36"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="37">
+        <f>SUM(J57:J63)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="31"/>
+      <c r="B65" s="31"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31"/>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B64" s="20"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="G64" s="40" t="s">
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="G66" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="H64" s="39"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="A65" s="5" t="s">
+      <c r="H66" s="41"/>
+      <c r="I66" s="41"/>
+      <c r="J66" s="41"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B67" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="12" t="s">
+      <c r="C67" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D65" s="12" t="s">
+      <c r="D67" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G65" s="17" t="s">
+      <c r="G67" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H65" s="17" t="s">
+      <c r="H67" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I65" s="17" t="s">
+      <c r="I67" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J67" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="J65" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="A66" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B66" s="4">
-        <f>Zusammenfassung!E2</f>
-        <v>0</v>
-      </c>
-      <c r="C66" s="6">
-        <v>3860</v>
-      </c>
-      <c r="D66" s="7">
-        <f>B66*C66</f>
-        <v>0</v>
-      </c>
-      <c r="G66" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H66" s="18">
-        <v>55</v>
-      </c>
-      <c r="I66" s="18">
-        <f>Zusammenfassung!F2-B66*15</f>
-        <v>0</v>
-      </c>
-      <c r="J66" s="18">
-        <f>H66*I66</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A67" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B67" s="4">
-        <f>Zusammenfassung!E3</f>
-        <v>0</v>
-      </c>
-      <c r="C67" s="6">
-        <v>3940</v>
-      </c>
-      <c r="D67" s="7">
-        <f t="shared" ref="D67:D72" si="4">B67*C67</f>
-        <v>0</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H67" s="18">
-        <v>61</v>
-      </c>
-      <c r="I67" s="18">
-        <f>Zusammenfassung!F3-B67*15</f>
-        <v>0</v>
-      </c>
-      <c r="J67" s="18">
-        <f t="shared" ref="J67:J72" si="5">H67*I67</f>
-        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B68" s="4">
-        <f>Zusammenfassung!E4</f>
+        <f>Zusammenfassung!E2</f>
         <v>0</v>
       </c>
       <c r="C68" s="6">
-        <v>4230</v>
+        <v>3860</v>
       </c>
       <c r="D68" s="7">
-        <f t="shared" si="4"/>
+        <f>B68*C68</f>
         <v>0</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H68" s="18">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="I68" s="18">
-        <f>Zusammenfassung!F4-B68*15</f>
+        <f>Zusammenfassung!F2-B68*15</f>
         <v>0</v>
       </c>
       <c r="J68" s="18">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+        <f>H68*I68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="14.25" customHeight="1">
       <c r="A69" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B69" s="4">
-        <f>Zusammenfassung!E5</f>
+        <f>Zusammenfassung!E3</f>
         <v>0</v>
       </c>
       <c r="C69" s="6">
-        <v>4950</v>
+        <v>3940</v>
       </c>
       <c r="D69" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D69:D74" si="4">B69*C69</f>
         <v>0</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H69" s="18">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="I69" s="18">
-        <f>Zusammenfassung!F5-B69*15</f>
+        <f>Zusammenfassung!F3-B69*15</f>
         <v>0</v>
       </c>
       <c r="J69" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="J69:J74" si="5">H69*I69</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B70" s="4">
-        <f>Zusammenfassung!E6</f>
+        <f>Zusammenfassung!E4</f>
         <v>0</v>
       </c>
       <c r="C70" s="6">
-        <v>6480</v>
+        <v>4230</v>
       </c>
       <c r="D70" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H70" s="18">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="I70" s="18">
-        <f>Zusammenfassung!F6-B70*15</f>
+        <f>Zusammenfassung!F4-B70*15</f>
         <v>0</v>
       </c>
       <c r="J70" s="18">
@@ -2487,27 +2470,27 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B71" s="4">
-        <f>Zusammenfassung!E7</f>
+        <f>Zusammenfassung!E5</f>
         <v>0</v>
       </c>
       <c r="C71" s="6">
-        <v>7480</v>
+        <v>4950</v>
       </c>
       <c r="D71" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H71" s="18">
-        <v>174</v>
+        <v>91</v>
       </c>
       <c r="I71" s="18">
-        <f>Zusammenfassung!F7-B71*15</f>
+        <f>Zusammenfassung!F5-B71*15</f>
         <v>0</v>
       </c>
       <c r="J71" s="18">
@@ -2517,27 +2500,27 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B72" s="4">
-        <f>Zusammenfassung!E8</f>
+        <f>Zusammenfassung!E6</f>
         <v>0</v>
       </c>
       <c r="C72" s="6">
-        <v>10020</v>
+        <v>6480</v>
       </c>
       <c r="D72" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H72" s="18">
-        <v>205</v>
+        <v>120</v>
       </c>
       <c r="I72" s="18">
-        <f>Zusammenfassung!F8-B72*15</f>
+        <f>Zusammenfassung!F6-B72*15</f>
         <v>0</v>
       </c>
       <c r="J72" s="18">
@@ -2547,161 +2530,221 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B73" s="4">
+        <f>Zusammenfassung!E7</f>
+        <v>0</v>
+      </c>
+      <c r="C73" s="6">
+        <v>7480</v>
+      </c>
+      <c r="D73" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H73" s="18">
+        <v>174</v>
+      </c>
+      <c r="I73" s="18">
+        <f>Zusammenfassung!F7-B73*15</f>
+        <v>0</v>
+      </c>
+      <c r="J73" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" s="4">
+        <f>Zusammenfassung!E8</f>
+        <v>0</v>
+      </c>
+      <c r="C74" s="6">
+        <v>10020</v>
+      </c>
+      <c r="D74" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H74" s="18">
+        <v>205</v>
+      </c>
+      <c r="I74" s="18">
+        <f>Zusammenfassung!F8-B74*15</f>
+        <v>0</v>
+      </c>
+      <c r="J74" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B73" s="4">
-        <f>SUM(B66:B72)</f>
-        <v>0</v>
-      </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="7">
-        <f>SUM(D66:D72)</f>
-        <v>0</v>
-      </c>
-      <c r="G73" s="4" t="s">
+      <c r="B75" s="4">
+        <f>SUM(B68:B74)</f>
+        <v>0</v>
+      </c>
+      <c r="C75" s="6"/>
+      <c r="D75" s="7">
+        <f>SUM(D68:D74)</f>
+        <v>0</v>
+      </c>
+      <c r="G75" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="18">
-        <f>SUM(J66:J72)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" s="51" t="s">
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="18">
+        <f>SUM(J68:J74)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B75" s="52"/>
-      <c r="C75" s="52"/>
-      <c r="D75" s="52"/>
-    </row>
-    <row r="86" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A86" s="9" t="s">
+      <c r="B77" s="54"/>
+      <c r="C77" s="54"/>
+      <c r="D77" s="54"/>
+    </row>
+    <row r="88" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A88" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="11"/>
-    </row>
-    <row r="87" spans="1:4" ht="60" customHeight="1">
-      <c r="A87" s="1" t="s">
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="11"/>
+    </row>
+    <row r="89" spans="1:4" ht="60" customHeight="1">
+      <c r="A89" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B87" s="12" t="s">
+      <c r="B89" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C87" s="12" t="s">
+      <c r="C89" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D87" s="12" t="s">
+      <c r="D89" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="8" t="s">
+    <row r="90" spans="1:4">
+      <c r="A90" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B88" s="4"/>
-      <c r="C88" s="6">
-        <v>0</v>
-      </c>
-      <c r="D88" s="7">
-        <f>B88*C88</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="31"/>
-      <c r="B89" s="31"/>
-      <c r="C89" s="31"/>
-      <c r="D89" s="31"/>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="13" t="s">
+      <c r="B90" s="4"/>
+      <c r="C90" s="6">
+        <v>0</v>
+      </c>
+      <c r="D90" s="7">
+        <f>B90*C90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="31"/>
+      <c r="B91" s="31"/>
+      <c r="C91" s="31"/>
+      <c r="D91" s="31"/>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B90" s="14"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="15"/>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="B91" s="60"/>
-      <c r="C91" s="60"/>
-      <c r="D91" s="60"/>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="61"/>
-      <c r="B92" s="61"/>
-      <c r="C92" s="61"/>
-      <c r="D92" s="61"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="15"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="61"/>
-      <c r="B93" s="61"/>
-      <c r="C93" s="61"/>
-      <c r="D93" s="61"/>
-    </row>
-    <row r="94" spans="1:4" ht="14.4" thickBot="1">
-      <c r="A94" s="61"/>
-      <c r="B94" s="61"/>
-      <c r="C94" s="61"/>
-      <c r="D94" s="61"/>
-    </row>
-    <row r="95" spans="1:4" ht="14.4" thickBot="1">
-      <c r="A95" s="14" t="s">
+      <c r="A93" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="B93" s="62"/>
+      <c r="C93" s="62"/>
+      <c r="D93" s="62"/>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="63"/>
+      <c r="B94" s="63"/>
+      <c r="C94" s="63"/>
+      <c r="D94" s="63"/>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="63"/>
+      <c r="B95" s="63"/>
+      <c r="C95" s="63"/>
+      <c r="D95" s="63"/>
+    </row>
+    <row r="96" spans="1:4" ht="14.4" thickBot="1">
+      <c r="A96" s="63"/>
+      <c r="B96" s="63"/>
+      <c r="C96" s="63"/>
+      <c r="D96" s="63"/>
+    </row>
+    <row r="97" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A97" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14"/>
+      <c r="D97" s="16">
+        <f>D32+D64+D90+J64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A98" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B95" s="14"/>
-      <c r="C95" s="14"/>
-      <c r="D95" s="16">
-        <f>D31+D62+D88+J62</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="14.4" thickBot="1">
-      <c r="A96" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B96" s="14"/>
-      <c r="C96" s="14"/>
-      <c r="D96" s="16">
-        <f>D48+D73+D88+J73</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="15" customHeight="1">
-      <c r="A100" s="44" t="s">
+      <c r="B98" s="14"/>
+      <c r="C98" s="14"/>
+      <c r="D98" s="16">
+        <f>D50+D75+D90+J75</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15" customHeight="1">
+      <c r="A102" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B100" s="44"/>
-      <c r="C100" s="44"/>
-      <c r="D100" s="44"/>
-      <c r="E100" s="44"/>
-    </row>
-    <row r="101" spans="1:5">
-      <c r="A101" s="44"/>
-      <c r="B101" s="44"/>
-      <c r="C101" s="44"/>
-      <c r="D101" s="44"/>
-      <c r="E101" s="44"/>
-    </row>
-    <row r="102" spans="1:5">
-      <c r="A102" s="44"/>
-      <c r="B102" s="44"/>
-      <c r="C102" s="44"/>
-      <c r="D102" s="44"/>
-      <c r="E102" s="44"/>
+      <c r="B102" s="46"/>
+      <c r="C102" s="46"/>
+      <c r="D102" s="46"/>
+      <c r="E102" s="46"/>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="44"/>
-      <c r="B103" s="44"/>
-      <c r="C103" s="44"/>
-      <c r="D103" s="44"/>
-      <c r="E103" s="44"/>
+      <c r="A103" s="46"/>
+      <c r="B103" s="46"/>
+      <c r="C103" s="46"/>
+      <c r="D103" s="46"/>
+      <c r="E103" s="46"/>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="46"/>
+      <c r="B104" s="46"/>
+      <c r="C104" s="46"/>
+      <c r="D104" s="46"/>
+      <c r="E104" s="46"/>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="46"/>
+      <c r="B105" s="46"/>
+      <c r="C105" s="46"/>
+      <c r="D105" s="46"/>
+      <c r="E105" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -2715,14 +2758,14 @@
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A9:E9"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="G64:J64"/>
+    <mergeCell ref="G55:J55"/>
+    <mergeCell ref="G66:J66"/>
     <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A100:E103"/>
-    <mergeCell ref="A50:E51"/>
-    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A102:E105"/>
+    <mergeCell ref="A52:E53"/>
+    <mergeCell ref="A77:D77"/>
     <mergeCell ref="A13:E14"/>
-    <mergeCell ref="A91:D94"/>
+    <mergeCell ref="A93:D96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2755,6 +2798,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101005FFC08842A22284F9348EB74BB1FFD7D" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="dce056f5060a025853d4b9bc213596f2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9f730088-dd1d-44a2-ba0b-9ee662212de1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6eeb49c5830c4bcc108e16c31212bcee" ns3:_="">
     <xsd:import namespace="9f730088-dd1d-44a2-ba0b-9ee662212de1"/>
@@ -2898,7 +2947,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2907,13 +2956,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE85EFE4-A7F1-4172-BE99-941086F215B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="9f730088-dd1d-44a2-ba0b-9ee662212de1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF99380-8091-4A51-9F6D-B6AAAB8AA62B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2931,26 +2990,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07D5089C-AFBA-4A9E-A982-3E0DC6ED90E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE85EFE4-A7F1-4172-BE99-941086F215B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="9f730088-dd1d-44a2-ba0b-9ee662212de1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>